<commit_message>
progress on finalizing CPFV
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb95/raw/Table28.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb95/raw/Table28.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb95/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBA145C-CD87-FC42-A715-26BBA215B942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79AE158-0B67-6345-AF71-1C88AB867330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Species</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>Salmon</t>
   </si>
 </sst>
 </file>
@@ -71,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -145,37 +148,37 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -493,17 +496,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +547,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -708,8 +711,10 @@
         <v>535832</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B6" s="10">
         <v>238</v>
       </c>
@@ -788,7 +793,7 @@
         <v>41043</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -870,7 +875,7 @@
         <v>1024978</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -952,7 +957,7 @@
         <v>587898</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>10</v>
       </c>

</xml_diff>